<commit_message>
work on progress bar and video page
</commit_message>
<xml_diff>
--- a/src/data/questions/Questionnaire for Upload.xlsx
+++ b/src/data/questions/Questionnaire for Upload.xlsx
@@ -10,22 +10,6 @@
   <definedNames/>
   <calcPr/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="B1">
-      <text>
-        <t xml:space="preserve">This is a unique identifier. It should be brief but readable, with no spaces
-	-Nick Oelsner</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11391,8 +11375,7 @@
       <formula1>"Workshop Eligibility,Basic Info,Waiver Flag,Red Flag"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11915,7 +11898,7 @@
         <f>English!E13</f>
         <v>radio</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>107</v>
       </c>
       <c r="G13" s="12" t="str">
@@ -12175,7 +12158,7 @@
         <f>English!E20</f>
         <v>radio</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="15" t="s">
         <v>107</v>
       </c>
       <c r="G20" s="12" t="str">
@@ -13055,7 +13038,7 @@
         <f>English!E44</f>
         <v/>
       </c>
-      <c r="F44" s="15"/>
+      <c r="F44" s="14"/>
       <c r="G44" s="12" t="str">
         <f>English!G44</f>
         <v/>
@@ -23987,7 +23970,7 @@
         <f>English!E3</f>
         <v>radio</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G3" s="12" t="str">
@@ -24366,7 +24349,7 @@
         <f>English!E13</f>
         <v>radio</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G13" s="12" t="str">
@@ -24403,7 +24386,7 @@
         <f>English!E14</f>
         <v>radio</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G14" s="12" t="str">
@@ -24478,7 +24461,7 @@
         <f>English!E16</f>
         <v>radio</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G16" s="12" t="str">
@@ -24515,7 +24498,7 @@
         <f>English!E17</f>
         <v>radio</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G17" s="12" t="str">
@@ -24552,7 +24535,7 @@
         <f>English!E18</f>
         <v>radio</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="str">
@@ -24589,7 +24572,7 @@
         <f>English!E19</f>
         <v>radio</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G19" s="12" t="str">
@@ -24626,7 +24609,7 @@
         <f>English!E20</f>
         <v>radio</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G20" s="12" t="str">
@@ -24663,7 +24646,7 @@
         <f>English!E21</f>
         <v>radio</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G21" s="12" t="str">
@@ -24738,7 +24721,7 @@
         <f>English!E23</f>
         <v>radio</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G23" s="12" t="str">
@@ -24775,7 +24758,7 @@
         <f>English!E24</f>
         <v>radio</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G24" s="12" t="str">
@@ -24812,7 +24795,7 @@
         <f>English!E25</f>
         <v>radio</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G25" s="12" t="str">
@@ -24849,7 +24832,7 @@
         <f>English!E26</f>
         <v>radio</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G26" s="12" t="str">
@@ -24886,7 +24869,7 @@
         <f>English!E27</f>
         <v>radio</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G27" s="12" t="str">
@@ -24923,7 +24906,7 @@
         <f>English!E28</f>
         <v>radio</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G28" s="12" t="str">
@@ -24960,7 +24943,7 @@
         <f>English!E29</f>
         <v>radio</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G29" s="12" t="str">
@@ -24997,7 +24980,7 @@
         <f>English!E30</f>
         <v>radio</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G30" s="12" t="str">
@@ -25034,7 +25017,7 @@
         <f>English!E31</f>
         <v>radio</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="12" t="str">
@@ -25071,7 +25054,7 @@
         <f>English!E32</f>
         <v>radio</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G32" s="12" t="str">
@@ -25108,7 +25091,7 @@
         <f>English!E33</f>
         <v>radio</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G33" s="12" t="str">
@@ -25145,7 +25128,7 @@
         <f>English!E34</f>
         <v>radio</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G34" s="12" t="str">
@@ -25182,7 +25165,7 @@
         <f>English!E35</f>
         <v>radio</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G35" s="12" t="str">
@@ -25219,7 +25202,7 @@
         <f>English!E36</f>
         <v>radio</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G36" s="12" t="str">
@@ -25256,7 +25239,7 @@
         <f>English!E37</f>
         <v>radio</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G37" s="12" t="str">
@@ -25293,7 +25276,7 @@
         <f>English!E38</f>
         <v>radio</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G38" s="12" t="str">
@@ -25330,7 +25313,7 @@
         <f>English!E39</f>
         <v>radio</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G39" s="12" t="str">
@@ -25367,7 +25350,7 @@
         <f>English!E40</f>
         <v>radio</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G40" s="12" t="str">

</xml_diff>

<commit_message>
add progress bar to top of questionnaire page
</commit_message>
<xml_diff>
--- a/src/data/questions/Questionnaire for Upload.xlsx
+++ b/src/data/questions/Questionnaire for Upload.xlsx
@@ -10,22 +10,6 @@
   <definedNames/>
   <calcPr/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="B1">
-      <text>
-        <t xml:space="preserve">This is a unique identifier. It should be brief but readable, with no spaces
-	-Nick Oelsner</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11391,8 +11375,7 @@
       <formula1>"Workshop Eligibility,Basic Info,Waiver Flag,Red Flag"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11915,7 +11898,7 @@
         <f>English!E13</f>
         <v>radio</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>107</v>
       </c>
       <c r="G13" s="12" t="str">
@@ -12175,7 +12158,7 @@
         <f>English!E20</f>
         <v>radio</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="15" t="s">
         <v>107</v>
       </c>
       <c r="G20" s="12" t="str">
@@ -13055,7 +13038,7 @@
         <f>English!E44</f>
         <v/>
       </c>
-      <c r="F44" s="15"/>
+      <c r="F44" s="14"/>
       <c r="G44" s="12" t="str">
         <f>English!G44</f>
         <v/>
@@ -23987,7 +23970,7 @@
         <f>English!E3</f>
         <v>radio</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G3" s="12" t="str">
@@ -24366,7 +24349,7 @@
         <f>English!E13</f>
         <v>radio</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G13" s="12" t="str">
@@ -24403,7 +24386,7 @@
         <f>English!E14</f>
         <v>radio</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G14" s="12" t="str">
@@ -24478,7 +24461,7 @@
         <f>English!E16</f>
         <v>radio</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G16" s="12" t="str">
@@ -24515,7 +24498,7 @@
         <f>English!E17</f>
         <v>radio</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G17" s="12" t="str">
@@ -24552,7 +24535,7 @@
         <f>English!E18</f>
         <v>radio</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="str">
@@ -24589,7 +24572,7 @@
         <f>English!E19</f>
         <v>radio</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G19" s="12" t="str">
@@ -24626,7 +24609,7 @@
         <f>English!E20</f>
         <v>radio</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G20" s="12" t="str">
@@ -24663,7 +24646,7 @@
         <f>English!E21</f>
         <v>radio</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G21" s="12" t="str">
@@ -24738,7 +24721,7 @@
         <f>English!E23</f>
         <v>radio</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G23" s="12" t="str">
@@ -24775,7 +24758,7 @@
         <f>English!E24</f>
         <v>radio</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G24" s="12" t="str">
@@ -24812,7 +24795,7 @@
         <f>English!E25</f>
         <v>radio</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G25" s="12" t="str">
@@ -24849,7 +24832,7 @@
         <f>English!E26</f>
         <v>radio</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G26" s="12" t="str">
@@ -24886,7 +24869,7 @@
         <f>English!E27</f>
         <v>radio</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G27" s="12" t="str">
@@ -24923,7 +24906,7 @@
         <f>English!E28</f>
         <v>radio</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G28" s="12" t="str">
@@ -24960,7 +24943,7 @@
         <f>English!E29</f>
         <v>radio</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G29" s="12" t="str">
@@ -24997,7 +24980,7 @@
         <f>English!E30</f>
         <v>radio</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G30" s="12" t="str">
@@ -25034,7 +25017,7 @@
         <f>English!E31</f>
         <v>radio</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="12" t="str">
@@ -25071,7 +25054,7 @@
         <f>English!E32</f>
         <v>radio</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G32" s="12" t="str">
@@ -25108,7 +25091,7 @@
         <f>English!E33</f>
         <v>radio</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G33" s="12" t="str">
@@ -25145,7 +25128,7 @@
         <f>English!E34</f>
         <v>radio</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G34" s="12" t="str">
@@ -25182,7 +25165,7 @@
         <f>English!E35</f>
         <v>radio</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G35" s="12" t="str">
@@ -25219,7 +25202,7 @@
         <f>English!E36</f>
         <v>radio</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G36" s="12" t="str">
@@ -25256,7 +25239,7 @@
         <f>English!E37</f>
         <v>radio</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G37" s="12" t="str">
@@ -25293,7 +25276,7 @@
         <f>English!E38</f>
         <v>radio</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G38" s="12" t="str">
@@ -25330,7 +25313,7 @@
         <f>English!E39</f>
         <v>radio</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G39" s="12" t="str">
@@ -25367,7 +25350,7 @@
         <f>English!E40</f>
         <v>radio</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G40" s="12" t="str">

</xml_diff>